<commit_message>
Diagrama de Afinidades e peso do product backlog
</commit_message>
<xml_diff>
--- a/Documentacao/ProductBacklog.xlsx
+++ b/Documentacao/ProductBacklog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukki\Desktop\Facul\AutopecasMcQueen\Documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\@ssoyjoo\Projeto Final\AutopecasMcQueen\Documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A631D851-D333-4A3F-8EF1-D3B8D1E1A6F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEFC0651-414E-46C4-8353-9728830540CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="3" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="46">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -82,9 +82,6 @@
     <t>Registro de despesas</t>
   </si>
   <si>
-    <t>Visualização de lançamentos</t>
-  </si>
-  <si>
     <t>Cadastro de fornecedores</t>
   </si>
   <si>
@@ -161,6 +158,18 @@
   </si>
   <si>
     <t>Peso (1 a 10)</t>
+  </si>
+  <si>
+    <t>Nota Fiscal</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Registro de lançamentos</t>
+  </si>
+  <si>
+    <t>10</t>
   </si>
 </sst>
 </file>
@@ -217,7 +226,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -242,8 +251,101 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top/>
@@ -259,10 +361,19 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -272,70 +383,21 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -344,10 +406,10 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
+      <right style="medium">
         <color indexed="64"/>
       </right>
       <top/>
@@ -357,23 +419,8 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <left/>
+      <right/>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -384,59 +431,69 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -722,300 +779,359 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB9C6368-A51D-4C29-8F2B-5565314B4ED9}">
-  <dimension ref="B1:F23"/>
+  <dimension ref="B1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H13" activeCellId="1" sqref="B12 H13"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="1"/>
-    <col min="2" max="2" width="34.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" style="8" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="1"/>
+    <col min="2" max="2" width="34.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" style="8" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="1"/>
+    <col min="7" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="B2" s="16" t="s">
+    <row r="1" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="18"/>
-    </row>
-    <row r="3" spans="2:6" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="20"/>
+    </row>
+    <row r="3" spans="2:10" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="20" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="20" t="s">
-        <v>24</v>
-      </c>
-      <c r="F3" s="13" t="s">
+      <c r="D3" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="12" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="21">
+      <c r="D4" s="16">
         <v>6</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="16">
         <v>7</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="16">
         <v>7</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="16">
         <v>8</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="F7" s="14" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="21"/>
+      <c r="D8" s="16">
+        <v>6</v>
+      </c>
       <c r="E8" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="D9" s="21"/>
+      <c r="D9" s="16">
+        <v>9</v>
+      </c>
       <c r="E9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="21"/>
+      <c r="D10" s="16">
+        <v>2</v>
+      </c>
       <c r="E10" s="9" t="s">
-        <v>31</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="D11" s="21"/>
-      <c r="E11" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="D11" s="16">
+        <v>5</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B12" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="21"/>
+      <c r="D12" s="16">
+        <v>8</v>
+      </c>
       <c r="E12" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B13" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D13" s="21"/>
-      <c r="E13" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="14" t="s">
+      <c r="D13" s="16">
+        <v>8</v>
+      </c>
+      <c r="E13" s="11" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="F13" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B14" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="21"/>
+      <c r="D14" s="16">
+        <v>10</v>
+      </c>
       <c r="E14" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B15" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="21"/>
+      <c r="D15" s="16">
+        <v>4</v>
+      </c>
       <c r="E15" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="14" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B16" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="21"/>
+      <c r="D16" s="16">
+        <v>7</v>
+      </c>
       <c r="E16" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16" s="14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B17" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="21"/>
+      <c r="D17" s="16">
+        <v>4</v>
+      </c>
       <c r="E17" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17" s="14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18" s="4" t="s">
-        <v>16</v>
+        <v>44</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="21"/>
+      <c r="D18" s="16">
+        <v>4</v>
+      </c>
       <c r="E18" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="16">
+        <v>7</v>
+      </c>
+      <c r="E19" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" ht="14.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="5" t="s">
+      <c r="F19" s="13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" s="23"/>
+      <c r="D20" s="16">
+        <v>7</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="17">
         <v>9</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D19" s="22"/>
-      <c r="E19" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F19" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="E23" s="10"/>
+      <c r="E21" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="F21" s="26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E24" s="10"/>
     </row>
   </sheetData>
   <autoFilter ref="B3:F19" xr:uid="{AB9C6368-A51D-4C29-8F2B-5565314B4ED9}">
@@ -1028,7 +1144,7 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C19 D19" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C21" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Muito Alta,Alta,Média,Baixa,Muito Baixa"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1043,7 +1159,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
atualização do product backlog
</commit_message>
<xml_diff>
--- a/Documentacao/ProductBacklog.xlsx
+++ b/Documentacao/ProductBacklog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\@ssoyjoo\Projeto Final\AutopecasMcQueen\Documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEFC0651-414E-46C4-8353-9728830540CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CADCA36B-B083-49FE-A094-C2800F85A4F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Planilha2" sheetId="4" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$B$3:$F$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$B$3:$F$31</definedName>
   </definedNames>
   <calcPr calcId="0" calcOnSave="0"/>
   <extLst>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="58">
   <si>
     <t>Product Backlog</t>
   </si>
@@ -170,6 +170,42 @@
   </si>
   <si>
     <t>10</t>
+  </si>
+  <si>
+    <t>Grupos e temas</t>
+  </si>
+  <si>
+    <t>Documentação do projeto APSI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atualização do termo de Abertura do Projeto </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Análise dos Stakeholders </t>
+  </si>
+  <si>
+    <t>Definição de papéis do time Scrum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Protótipo v1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagrama de afinidades </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Proposta de melhorias </t>
+  </si>
+  <si>
+    <t>Protótipo v2</t>
+  </si>
+  <si>
+    <t>Projeto fisico do banco de dados</t>
+  </si>
+  <si>
+    <t>Documentação atualizada</t>
+  </si>
+  <si>
+    <t>Avaliação 360 graus - v1</t>
   </si>
 </sst>
 </file>
@@ -470,15 +506,6 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -494,6 +521,15 @@
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -779,10 +815,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB9C6368-A51D-4C29-8F2B-5565314B4ED9}">
-  <dimension ref="B1:J24"/>
+  <dimension ref="B1:J36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G30" sqref="D30:G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -796,17 +832,17 @@
     <col min="7" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B2" s="18" t="s">
+    <row r="1" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="20"/>
-    </row>
-    <row r="3" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="26"/>
+    </row>
+    <row r="3" spans="2:6" ht="15" x14ac:dyDescent="0.25">
       <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
@@ -823,9 +859,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>3</v>
@@ -840,303 +876,507 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B5" s="3" t="s">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" s="16">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B6" s="3" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>3</v>
       </c>
       <c r="D6" s="16">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B7" s="3" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>3</v>
       </c>
       <c r="D7" s="16">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E7" s="9" t="s">
         <v>29</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B8" s="4" t="s">
-        <v>14</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="16">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E8" s="9" t="s">
         <v>24</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D9" s="16">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
-        <v>19</v>
+        <v>51</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D10" s="16">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B11" s="4" t="s">
-        <v>13</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="16">
-        <v>5</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>28</v>
+        <v>7</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>24</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B12" s="4" t="s">
-        <v>15</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D12" s="16">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>24</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B13" s="4" t="s">
-        <v>12</v>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D13" s="16">
         <v>8</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="16">
+        <v>6</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="16">
+        <v>6</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="16">
+        <v>9</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="16">
+        <v>2</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B18" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="16">
+        <v>5</v>
+      </c>
+      <c r="E18" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F13" s="13" t="s">
+      <c r="F18" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B19" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="16">
+        <v>5</v>
+      </c>
+      <c r="E19" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F19" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B20" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="16">
+        <v>5</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F20" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B21" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="16">
+        <v>5</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B22" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="16">
+        <v>8</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B23" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="16">
+        <v>8</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F23" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="J13" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B14" s="4" t="s">
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B24" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" s="16">
+        <v>8</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B25" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" s="16">
+        <v>8</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B26" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C26" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D14" s="16">
+      <c r="D26" s="16">
         <v>10</v>
       </c>
-      <c r="E14" s="9" t="s">
+      <c r="E26" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F26" s="13" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B15" s="3" t="s">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B27" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C27" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D15" s="16">
+      <c r="D27" s="16">
         <v>4</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E27" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="F27" s="13" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B16" s="4" t="s">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B28" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C28" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D16" s="16">
+      <c r="D28" s="16">
         <v>7</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E28" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="13" t="s">
+      <c r="F28" s="13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B17" s="4" t="s">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B29" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C29" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D17" s="16">
+      <c r="D29" s="16">
         <v>4</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E29" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F29" s="13" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B18" s="4" t="s">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B30" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C30" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="16">
+      <c r="D30" s="16">
         <v>4</v>
       </c>
-      <c r="E18" s="9" t="s">
+      <c r="E30" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="F18" s="13" t="s">
+      <c r="F30" s="13" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B19" s="22" t="s">
+    <row r="31" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B31" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C31" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="16">
+      <c r="D31" s="16">
         <v>7</v>
       </c>
-      <c r="E19" s="24" t="s">
+      <c r="E31" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="F19" s="13" t="s">
+      <c r="F31" s="13" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B20" s="22" t="s">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B32" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="16">
+      <c r="C32" s="20"/>
+      <c r="D32" s="16">
         <v>7</v>
       </c>
-      <c r="E20" s="21" t="s">
+      <c r="E32" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="13" t="s">
+      <c r="F32" s="13" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="5" t="s">
+    <row r="33" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C33" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="17">
+      <c r="D33" s="17">
         <v>9</v>
       </c>
-      <c r="E21" s="25" t="s">
+      <c r="E33" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F21" s="26" t="s">
+      <c r="F33" s="23" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="E24" s="10"/>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="E36" s="10"/>
     </row>
   </sheetData>
-  <autoFilter ref="B3:F19" xr:uid="{AB9C6368-A51D-4C29-8F2B-5565314B4ED9}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:F19">
-      <sortCondition ref="F3:F19"/>
+  <autoFilter ref="B3:F31" xr:uid="{AB9C6368-A51D-4C29-8F2B-5565314B4ED9}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:F31">
+      <sortCondition ref="F3:F31"/>
     </sortState>
   </autoFilter>
   <mergeCells count="1">
@@ -1144,7 +1384,7 @@
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C21" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4:C33" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Muito Alta,Alta,Média,Baixa,Muito Baixa"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>